<commit_message>
add tables to .docx file
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="207">
   <si>
     <t xml:space="preserve">Unidade</t>
   </si>
@@ -237,13 +237,241 @@
     <t xml:space="preserve">Dedicado</t>
   </si>
   <si>
+    <t xml:space="preserve">TPLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLSG1048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cisco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2960-X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2960-S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3560G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruckus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R610</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZD3025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mais de 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">115200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BR DIGITAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SonicWall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSA5650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ckp </t>
+  </si>
+  <si>
     <t xml:space="preserve">802.11g;802.11n;802.11ac;</t>
   </si>
   <si>
+    <t xml:space="preserve">2960-BR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2960-POE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">até 10000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BR Digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next Generation Firewall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TZ600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cisco </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLSG1049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TZ300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pfsense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2961-X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRDIGITAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSA4650</t>
+  </si>
+  <si>
     <t xml:space="preserve">ADSL</t>
   </si>
   <si>
+    <t xml:space="preserve">zd3025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRdigital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">palo alto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2960BR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSA 2650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BR-Digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2962-X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BR-DIgital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HENET</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ​NSA 2650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3Com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3Com 3C17300A-4200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3Com 226 SFP PLUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-LINK 1210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubiquiti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIFI AP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unifi Controller em Virtual Machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Não especificado no utilização em Virtual Machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">até 1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SITELBRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firewall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PFSense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PFSense 2.4.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIBERCONECTIVIDADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TL-SF1024D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Não existe Firewall</t>
+  </si>
+  <si>
     <t xml:space="preserve">802.11b;802.11g;802.11n;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-Link DES 3526 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP V1910 48G </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UniFi Controller em Virtual Machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intelbras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SF2400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WANTEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BR-DIGITAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-LINK 1210 48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch 2226 SFP Plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOCALNET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INFORNET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILSYSTEM</t>
   </si>
   <si>
     <t xml:space="preserve">Estado</t>
@@ -549,7 +777,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -588,6 +816,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -685,16 +917,16 @@
   </sheetPr>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.03"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1457,11 +1689,11 @@
   </sheetPr>
   <dimension ref="A1:CV27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="30.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="9.32"/>
@@ -1472,6 +1704,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="9" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="13.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,36 +1735,93 @@
         <v>84</v>
       </c>
       <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
-      <c r="AO1" s="8"/>
+      <c r="J1" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="K1" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="L1" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="M1" s="7" t="n">
+        <v>19</v>
+      </c>
+      <c r="N1" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="O1" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="P1" s="7" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="7" t="n">
+        <v>28</v>
+      </c>
+      <c r="R1" s="7" t="n">
+        <v>32</v>
+      </c>
+      <c r="S1" s="7" t="n">
+        <v>33</v>
+      </c>
+      <c r="T1" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="U1" s="7" t="n">
+        <v>37</v>
+      </c>
+      <c r="V1" s="7" t="n">
+        <v>43</v>
+      </c>
+      <c r="W1" s="7" t="n">
+        <v>44</v>
+      </c>
+      <c r="X1" s="7" t="n">
+        <v>45</v>
+      </c>
+      <c r="Y1" s="7" t="n">
+        <v>64</v>
+      </c>
+      <c r="Z1" s="7" t="n">
+        <v>65</v>
+      </c>
+      <c r="AA1" s="7" t="n">
+        <v>70</v>
+      </c>
+      <c r="AB1" s="7" t="n">
+        <v>71</v>
+      </c>
+      <c r="AC1" s="7" t="n">
+        <v>72</v>
+      </c>
+      <c r="AD1" s="7" t="n">
+        <v>73</v>
+      </c>
+      <c r="AE1" s="7" t="n">
+        <v>74</v>
+      </c>
+      <c r="AF1" s="7" t="n">
+        <v>80</v>
+      </c>
+      <c r="AG1" s="7" t="n">
+        <v>83</v>
+      </c>
+      <c r="AH1" s="7" t="n">
+        <v>85</v>
+      </c>
+      <c r="AI1" s="7" t="n">
+        <v>88</v>
+      </c>
+      <c r="AJ1" s="7" t="n">
+        <v>89</v>
+      </c>
+      <c r="AK1" s="7" t="n">
+        <v>90</v>
+      </c>
+      <c r="AL1" s="7" t="n">
+        <v>97</v>
+      </c>
       <c r="AP1" s="8"/>
       <c r="AQ1" s="8"/>
       <c r="AR1" s="8"/>
@@ -1611,36 +1903,91 @@
         <v>15</v>
       </c>
       <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
-      <c r="AO2" s="9"/>
+      <c r="J2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="M2" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P2" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="T2" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="U2" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="X2" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC2" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF2" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG2" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH2" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL2" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="AP2" s="9"/>
       <c r="AQ2" s="9"/>
       <c r="AR2" s="9"/>
@@ -1659,8 +2006,8 @@
       <c r="BF2" s="9"/>
       <c r="BG2" s="9"/>
       <c r="BH2" s="9"/>
-      <c r="BI2" s="10"/>
-      <c r="BJ2" s="10"/>
+      <c r="BI2" s="11"/>
+      <c r="BJ2" s="11"/>
       <c r="BK2" s="9"/>
       <c r="BL2" s="9"/>
       <c r="BM2" s="9"/>
@@ -1672,16 +2019,16 @@
       <c r="BT2" s="9"/>
       <c r="BU2" s="9"/>
       <c r="BV2" s="9"/>
-      <c r="BW2" s="10"/>
-      <c r="BX2" s="10"/>
-      <c r="BY2" s="10"/>
+      <c r="BW2" s="11"/>
+      <c r="BX2" s="11"/>
+      <c r="BY2" s="11"/>
       <c r="CB2" s="9"/>
       <c r="CC2" s="9"/>
       <c r="CD2" s="9"/>
       <c r="CE2" s="9"/>
       <c r="CG2" s="9"/>
       <c r="CH2" s="9"/>
-      <c r="CI2" s="10"/>
+      <c r="CI2" s="11"/>
       <c r="CJ2" s="9"/>
       <c r="CK2" s="9"/>
       <c r="CL2" s="9"/>
@@ -1710,7 +2057,7 @@
         <v>67</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>70</v>
@@ -1722,36 +2069,83 @@
         <v>100</v>
       </c>
       <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="9"/>
-      <c r="AH3" s="9"/>
-      <c r="AI3" s="9"/>
-      <c r="AK3" s="9"/>
-      <c r="AM3" s="9"/>
-      <c r="AN3" s="9"/>
-      <c r="AO3" s="9"/>
+      <c r="J3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="P3" s="10" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="T3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U3" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE3" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF3" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="10"/>
+      <c r="AI3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ3" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK3" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL3" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="AP3" s="9"/>
       <c r="AQ3" s="9"/>
       <c r="AR3" s="9"/>
@@ -1770,8 +2164,8 @@
       <c r="BF3" s="9"/>
       <c r="BG3" s="9"/>
       <c r="BH3" s="9"/>
-      <c r="BI3" s="10"/>
-      <c r="BJ3" s="10"/>
+      <c r="BI3" s="11"/>
+      <c r="BJ3" s="11"/>
       <c r="BK3" s="9"/>
       <c r="BL3" s="9"/>
       <c r="BM3" s="9"/>
@@ -1783,16 +2177,16 @@
       <c r="BT3" s="9"/>
       <c r="BU3" s="9"/>
       <c r="BV3" s="9"/>
-      <c r="BW3" s="10"/>
-      <c r="BX3" s="10"/>
-      <c r="BY3" s="10"/>
+      <c r="BW3" s="11"/>
+      <c r="BX3" s="11"/>
+      <c r="BY3" s="11"/>
       <c r="CB3" s="9"/>
       <c r="CC3" s="9"/>
       <c r="CD3" s="9"/>
       <c r="CE3" s="9"/>
       <c r="CG3" s="9"/>
       <c r="CH3" s="9"/>
-      <c r="CI3" s="10"/>
+      <c r="CI3" s="11"/>
       <c r="CJ3" s="9"/>
       <c r="CK3" s="9"/>
       <c r="CL3" s="9"/>
@@ -1821,7 +2215,7 @@
         <v>67</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>70</v>
@@ -1833,36 +2227,79 @@
         <v>500</v>
       </c>
       <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
-      <c r="AH4" s="9"/>
-      <c r="AI4" s="9"/>
-      <c r="AK4" s="9"/>
-      <c r="AM4" s="9"/>
-      <c r="AN4" s="9"/>
-      <c r="AO4" s="9"/>
+      <c r="J4" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="P4" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="T4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z4" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC4" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD4" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF4" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG4" s="10"/>
+      <c r="AH4" s="10"/>
+      <c r="AI4" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ4" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL4" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="AP4" s="9"/>
       <c r="AQ4" s="9"/>
       <c r="AR4" s="9"/>
@@ -1881,8 +2318,8 @@
       <c r="BF4" s="9"/>
       <c r="BG4" s="9"/>
       <c r="BH4" s="9"/>
-      <c r="BI4" s="10"/>
-      <c r="BJ4" s="10"/>
+      <c r="BI4" s="11"/>
+      <c r="BJ4" s="11"/>
       <c r="BK4" s="9"/>
       <c r="BL4" s="9"/>
       <c r="BM4" s="9"/>
@@ -1894,16 +2331,16 @@
       <c r="BT4" s="9"/>
       <c r="BU4" s="9"/>
       <c r="BV4" s="9"/>
-      <c r="BW4" s="10"/>
-      <c r="BX4" s="10"/>
-      <c r="BY4" s="10"/>
+      <c r="BW4" s="11"/>
+      <c r="BX4" s="11"/>
+      <c r="BY4" s="11"/>
       <c r="CB4" s="9"/>
       <c r="CC4" s="9"/>
       <c r="CD4" s="9"/>
       <c r="CE4" s="9"/>
       <c r="CG4" s="9"/>
       <c r="CH4" s="9"/>
-      <c r="CI4" s="10"/>
+      <c r="CI4" s="11"/>
       <c r="CJ4" s="9"/>
       <c r="CK4" s="9"/>
       <c r="CL4" s="9"/>
@@ -1930,7 +2367,7 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>70</v>
@@ -1940,36 +2377,89 @@
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="9"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="9"/>
-      <c r="AI5" s="9"/>
-      <c r="AK5" s="9"/>
-      <c r="AM5" s="9"/>
-      <c r="AN5" s="9"/>
-      <c r="AO5" s="9"/>
+      <c r="J5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P5" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T5" s="10" t="n">
+        <v>27</v>
+      </c>
+      <c r="U5" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="W5" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="X5" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA5" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB5" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC5" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD5" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF5" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH5" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI5" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ5" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK5" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AL5" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="AP5" s="9"/>
       <c r="AQ5" s="9"/>
       <c r="AR5" s="9"/>
@@ -1988,8 +2478,8 @@
       <c r="BF5" s="9"/>
       <c r="BG5" s="9"/>
       <c r="BH5" s="9"/>
-      <c r="BI5" s="10"/>
-      <c r="BJ5" s="10"/>
+      <c r="BI5" s="11"/>
+      <c r="BJ5" s="11"/>
       <c r="BK5" s="9"/>
       <c r="BL5" s="9"/>
       <c r="BM5" s="9"/>
@@ -2001,16 +2491,16 @@
       <c r="BT5" s="9"/>
       <c r="BU5" s="9"/>
       <c r="BV5" s="9"/>
-      <c r="BW5" s="10"/>
-      <c r="BX5" s="10"/>
-      <c r="BY5" s="10"/>
+      <c r="BW5" s="11"/>
+      <c r="BX5" s="11"/>
+      <c r="BY5" s="11"/>
       <c r="CB5" s="9"/>
       <c r="CC5" s="9"/>
       <c r="CD5" s="9"/>
       <c r="CE5" s="9"/>
       <c r="CG5" s="9"/>
       <c r="CH5" s="9"/>
-      <c r="CI5" s="10"/>
+      <c r="CI5" s="11"/>
       <c r="CJ5" s="9"/>
       <c r="CK5" s="9"/>
       <c r="CL5" s="9"/>
@@ -2037,46 +2527,103 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="G6" s="4" t="n">
         <v>25</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="9"/>
-      <c r="AF6" s="9"/>
-      <c r="AG6" s="9"/>
-      <c r="AH6" s="9"/>
-      <c r="AI6" s="9"/>
-      <c r="AK6" s="9"/>
-      <c r="AM6" s="9"/>
-      <c r="AN6" s="9"/>
-      <c r="AO6" s="9"/>
+      <c r="J6" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="M6" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="P6" s="10" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="T6" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="U6" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V6" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="W6" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="X6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z6" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA6" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB6" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC6" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD6" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF6" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH6" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI6" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ6" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK6" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AL6" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="AP6" s="9"/>
       <c r="AQ6" s="9"/>
       <c r="AR6" s="9"/>
@@ -2095,8 +2642,8 @@
       <c r="BF6" s="9"/>
       <c r="BG6" s="9"/>
       <c r="BH6" s="9"/>
-      <c r="BI6" s="10"/>
-      <c r="BJ6" s="10"/>
+      <c r="BI6" s="11"/>
+      <c r="BJ6" s="11"/>
       <c r="BK6" s="9"/>
       <c r="BL6" s="9"/>
       <c r="BM6" s="9"/>
@@ -2108,16 +2655,16 @@
       <c r="BT6" s="9"/>
       <c r="BU6" s="9"/>
       <c r="BV6" s="9"/>
-      <c r="BW6" s="10"/>
-      <c r="BX6" s="10"/>
-      <c r="BY6" s="10"/>
+      <c r="BW6" s="11"/>
+      <c r="BX6" s="11"/>
+      <c r="BY6" s="11"/>
       <c r="CB6" s="9"/>
       <c r="CC6" s="9"/>
       <c r="CD6" s="9"/>
       <c r="CE6" s="9"/>
       <c r="CG6" s="9"/>
       <c r="CH6" s="9"/>
-      <c r="CI6" s="10"/>
+      <c r="CI6" s="11"/>
       <c r="CJ6" s="9"/>
       <c r="CK6" s="9"/>
       <c r="CL6" s="9"/>
@@ -2146,7 +2693,7 @@
         <v>67</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>70</v>
@@ -2158,36 +2705,93 @@
         <v>100</v>
       </c>
       <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
-      <c r="AF7" s="9"/>
-      <c r="AG7" s="9"/>
-      <c r="AH7" s="9"/>
-      <c r="AI7" s="9"/>
-      <c r="AK7" s="9"/>
-      <c r="AM7" s="9"/>
-      <c r="AN7" s="9"/>
-      <c r="AO7" s="9"/>
+      <c r="J7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="L7" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="P7" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="T7" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="U7" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="X7" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z7" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA7" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC7" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD7" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE7" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF7" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG7" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH7" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI7" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ7" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK7" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AL7" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="AP7" s="9"/>
       <c r="AQ7" s="9"/>
       <c r="AR7" s="9"/>
@@ -2206,8 +2810,8 @@
       <c r="BF7" s="9"/>
       <c r="BG7" s="9"/>
       <c r="BH7" s="9"/>
-      <c r="BI7" s="10"/>
-      <c r="BJ7" s="10"/>
+      <c r="BI7" s="11"/>
+      <c r="BJ7" s="11"/>
       <c r="BK7" s="9"/>
       <c r="BL7" s="9"/>
       <c r="BM7" s="9"/>
@@ -2219,16 +2823,16 @@
       <c r="BT7" s="9"/>
       <c r="BU7" s="9"/>
       <c r="BV7" s="9"/>
-      <c r="BW7" s="10"/>
-      <c r="BX7" s="10"/>
-      <c r="BY7" s="10"/>
+      <c r="BW7" s="11"/>
+      <c r="BX7" s="11"/>
+      <c r="BY7" s="11"/>
       <c r="CB7" s="9"/>
       <c r="CC7" s="9"/>
       <c r="CD7" s="9"/>
       <c r="CE7" s="9"/>
       <c r="CG7" s="9"/>
       <c r="CH7" s="9"/>
-      <c r="CI7" s="10"/>
+      <c r="CI7" s="11"/>
       <c r="CJ7" s="9"/>
       <c r="CK7" s="9"/>
       <c r="CL7" s="9"/>
@@ -2257,7 +2861,7 @@
         <v>67</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>70</v>
@@ -2269,36 +2873,79 @@
         <v>25</v>
       </c>
       <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="9"/>
-      <c r="AF8" s="9"/>
-      <c r="AG8" s="9"/>
-      <c r="AH8" s="9"/>
-      <c r="AI8" s="9"/>
-      <c r="AK8" s="9"/>
-      <c r="AM8" s="9"/>
-      <c r="AN8" s="9"/>
-      <c r="AO8" s="9"/>
+      <c r="J8" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="P8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R8" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S8" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U8" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z8" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA8" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB8" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC8" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD8" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE8" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF8" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="10"/>
+      <c r="AI8" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ8" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK8" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL8" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="AP8" s="9"/>
       <c r="AQ8" s="9"/>
       <c r="AR8" s="9"/>
@@ -2317,8 +2964,8 @@
       <c r="BF8" s="9"/>
       <c r="BG8" s="9"/>
       <c r="BH8" s="9"/>
-      <c r="BI8" s="10"/>
-      <c r="BJ8" s="10"/>
+      <c r="BI8" s="11"/>
+      <c r="BJ8" s="11"/>
       <c r="BK8" s="9"/>
       <c r="BL8" s="9"/>
       <c r="BM8" s="9"/>
@@ -2330,16 +2977,16 @@
       <c r="BT8" s="9"/>
       <c r="BU8" s="9"/>
       <c r="BV8" s="9"/>
-      <c r="BW8" s="10"/>
-      <c r="BX8" s="10"/>
-      <c r="BY8" s="10"/>
+      <c r="BW8" s="11"/>
+      <c r="BX8" s="11"/>
+      <c r="BY8" s="11"/>
       <c r="CB8" s="9"/>
       <c r="CC8" s="9"/>
       <c r="CD8" s="9"/>
       <c r="CE8" s="9"/>
       <c r="CG8" s="9"/>
       <c r="CH8" s="9"/>
-      <c r="CI8" s="10"/>
+      <c r="CI8" s="11"/>
       <c r="CJ8" s="9"/>
       <c r="CK8" s="9"/>
       <c r="CL8" s="9"/>
@@ -2366,7 +3013,7 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>70</v>
@@ -2376,36 +3023,83 @@
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
-      <c r="Y9" s="9"/>
-      <c r="Z9" s="9"/>
-      <c r="AA9" s="9"/>
-      <c r="AB9" s="9"/>
-      <c r="AC9" s="9"/>
-      <c r="AD9" s="9"/>
-      <c r="AE9" s="9"/>
-      <c r="AF9" s="9"/>
-      <c r="AG9" s="9"/>
-      <c r="AH9" s="9"/>
-      <c r="AI9" s="9"/>
-      <c r="AK9" s="9"/>
-      <c r="AM9" s="9"/>
-      <c r="AN9" s="9"/>
-      <c r="AO9" s="9"/>
+      <c r="J9" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P9" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T9" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="U9" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z9" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA9" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC9" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD9" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE9" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF9" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH9" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI9" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ9" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK9" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL9" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="AP9" s="9"/>
       <c r="AQ9" s="9"/>
       <c r="AR9" s="9"/>
@@ -2424,8 +3118,8 @@
       <c r="BF9" s="9"/>
       <c r="BG9" s="9"/>
       <c r="BH9" s="9"/>
-      <c r="BI9" s="10"/>
-      <c r="BJ9" s="10"/>
+      <c r="BI9" s="11"/>
+      <c r="BJ9" s="11"/>
       <c r="BK9" s="9"/>
       <c r="BL9" s="9"/>
       <c r="BM9" s="9"/>
@@ -2437,16 +3131,16 @@
       <c r="BT9" s="9"/>
       <c r="BU9" s="9"/>
       <c r="BV9" s="9"/>
-      <c r="BW9" s="10"/>
-      <c r="BX9" s="10"/>
-      <c r="BY9" s="10"/>
+      <c r="BW9" s="11"/>
+      <c r="BX9" s="11"/>
+      <c r="BY9" s="11"/>
       <c r="CB9" s="9"/>
       <c r="CC9" s="9"/>
       <c r="CD9" s="9"/>
       <c r="CE9" s="9"/>
       <c r="CG9" s="9"/>
       <c r="CH9" s="9"/>
-      <c r="CI9" s="10"/>
+      <c r="CI9" s="11"/>
       <c r="CJ9" s="9"/>
       <c r="CK9" s="9"/>
       <c r="CL9" s="9"/>
@@ -2473,7 +3167,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>70</v>
@@ -2485,36 +3179,79 @@
         <v>50</v>
       </c>
       <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="9"/>
-      <c r="AF10" s="9"/>
-      <c r="AG10" s="9"/>
-      <c r="AH10" s="9"/>
-      <c r="AI10" s="9"/>
-      <c r="AK10" s="9"/>
-      <c r="AM10" s="9"/>
-      <c r="AN10" s="9"/>
-      <c r="AO10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U10" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z10" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA10" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB10" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC10" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD10" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE10" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF10" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG10" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH10" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI10" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ10" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK10" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL10" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="AP10" s="9"/>
       <c r="AQ10" s="9"/>
       <c r="AR10" s="9"/>
@@ -2533,8 +3270,8 @@
       <c r="BF10" s="9"/>
       <c r="BG10" s="9"/>
       <c r="BH10" s="9"/>
-      <c r="BI10" s="10"/>
-      <c r="BJ10" s="10"/>
+      <c r="BI10" s="11"/>
+      <c r="BJ10" s="11"/>
       <c r="BK10" s="9"/>
       <c r="BL10" s="9"/>
       <c r="BM10" s="9"/>
@@ -2546,16 +3283,16 @@
       <c r="BT10" s="9"/>
       <c r="BU10" s="9"/>
       <c r="BV10" s="9"/>
-      <c r="BW10" s="10"/>
-      <c r="BX10" s="10"/>
-      <c r="BY10" s="10"/>
+      <c r="BW10" s="11"/>
+      <c r="BX10" s="11"/>
+      <c r="BY10" s="11"/>
       <c r="CB10" s="9"/>
       <c r="CC10" s="9"/>
       <c r="CD10" s="9"/>
       <c r="CE10" s="9"/>
       <c r="CG10" s="9"/>
       <c r="CH10" s="9"/>
-      <c r="CI10" s="10"/>
+      <c r="CI10" s="11"/>
       <c r="CJ10" s="9"/>
       <c r="CK10" s="9"/>
       <c r="CL10" s="9"/>
@@ -2582,7 +3319,7 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>70</v>
@@ -2594,36 +3331,79 @@
         <v>50</v>
       </c>
       <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="9"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="9"/>
-      <c r="AF11" s="9"/>
-      <c r="AG11" s="9"/>
-      <c r="AH11" s="9"/>
-      <c r="AI11" s="9"/>
-      <c r="AK11" s="9"/>
-      <c r="AM11" s="9"/>
-      <c r="AN11" s="9"/>
-      <c r="AO11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P11" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S11" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T11" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="U11" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z11" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA11" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC11" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD11" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE11" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF11" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG11" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH11" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI11" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ11" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK11" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL11" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="AP11" s="9"/>
       <c r="AQ11" s="9"/>
       <c r="AR11" s="9"/>
@@ -2642,8 +3422,8 @@
       <c r="BF11" s="9"/>
       <c r="BG11" s="9"/>
       <c r="BH11" s="9"/>
-      <c r="BI11" s="10"/>
-      <c r="BJ11" s="10"/>
+      <c r="BI11" s="11"/>
+      <c r="BJ11" s="11"/>
       <c r="BK11" s="9"/>
       <c r="BL11" s="9"/>
       <c r="BM11" s="9"/>
@@ -2655,16 +3435,16 @@
       <c r="BT11" s="9"/>
       <c r="BU11" s="9"/>
       <c r="BV11" s="9"/>
-      <c r="BW11" s="10"/>
-      <c r="BX11" s="10"/>
-      <c r="BY11" s="10"/>
+      <c r="BW11" s="11"/>
+      <c r="BX11" s="11"/>
+      <c r="BY11" s="11"/>
       <c r="CB11" s="9"/>
       <c r="CC11" s="9"/>
       <c r="CD11" s="9"/>
       <c r="CE11" s="9"/>
       <c r="CG11" s="9"/>
       <c r="CH11" s="9"/>
-      <c r="CI11" s="10"/>
+      <c r="CI11" s="11"/>
       <c r="CJ11" s="9"/>
       <c r="CK11" s="9"/>
       <c r="CL11" s="9"/>
@@ -2691,7 +3471,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>70</v>
@@ -2703,36 +3483,87 @@
         <v>50</v>
       </c>
       <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="9"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9"/>
-      <c r="AF12" s="9"/>
-      <c r="AG12" s="9"/>
-      <c r="AH12" s="9"/>
-      <c r="AI12" s="9"/>
-      <c r="AK12" s="9"/>
-      <c r="AM12" s="9"/>
-      <c r="AN12" s="9"/>
-      <c r="AO12" s="9"/>
+      <c r="J12" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="L12" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="M12" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="P12" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q12" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R12" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="S12" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="T12" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="U12" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z12" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB12" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC12" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD12" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE12" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF12" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="AG12" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH12" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI12" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="AJ12" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK12" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="AL12" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="AP12" s="9"/>
       <c r="AQ12" s="9"/>
       <c r="AR12" s="9"/>
@@ -2751,8 +3582,8 @@
       <c r="BF12" s="9"/>
       <c r="BG12" s="9"/>
       <c r="BH12" s="9"/>
-      <c r="BI12" s="10"/>
-      <c r="BJ12" s="10"/>
+      <c r="BI12" s="11"/>
+      <c r="BJ12" s="11"/>
       <c r="BK12" s="9"/>
       <c r="BL12" s="9"/>
       <c r="BM12" s="9"/>
@@ -2764,16 +3595,16 @@
       <c r="BT12" s="9"/>
       <c r="BU12" s="9"/>
       <c r="BV12" s="9"/>
-      <c r="BW12" s="10"/>
-      <c r="BX12" s="10"/>
-      <c r="BY12" s="10"/>
+      <c r="BW12" s="11"/>
+      <c r="BX12" s="11"/>
+      <c r="BY12" s="11"/>
       <c r="CB12" s="9"/>
       <c r="CC12" s="9"/>
       <c r="CD12" s="9"/>
       <c r="CE12" s="9"/>
       <c r="CG12" s="9"/>
       <c r="CH12" s="9"/>
-      <c r="CI12" s="10"/>
+      <c r="CI12" s="11"/>
       <c r="CJ12" s="9"/>
       <c r="CK12" s="9"/>
       <c r="CL12" s="9"/>
@@ -2800,7 +3631,7 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>70</v>
@@ -2812,36 +3643,79 @@
         <v>50</v>
       </c>
       <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="9"/>
-      <c r="AA13" s="9"/>
-      <c r="AB13" s="9"/>
-      <c r="AC13" s="9"/>
-      <c r="AD13" s="9"/>
-      <c r="AE13" s="9"/>
-      <c r="AF13" s="9"/>
-      <c r="AG13" s="9"/>
-      <c r="AH13" s="9"/>
-      <c r="AI13" s="9"/>
-      <c r="AK13" s="9"/>
-      <c r="AM13" s="9"/>
-      <c r="AN13" s="9"/>
-      <c r="AO13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P13" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S13" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T13" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="U13" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z13" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA13" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB13" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC13" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD13" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE13" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF13" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG13" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH13" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI13" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ13" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK13" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AL13" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="AP13" s="9"/>
       <c r="AQ13" s="9"/>
       <c r="AR13" s="9"/>
@@ -2860,8 +3734,8 @@
       <c r="BF13" s="9"/>
       <c r="BG13" s="9"/>
       <c r="BH13" s="9"/>
-      <c r="BI13" s="10"/>
-      <c r="BJ13" s="10"/>
+      <c r="BI13" s="11"/>
+      <c r="BJ13" s="11"/>
       <c r="BK13" s="9"/>
       <c r="BL13" s="9"/>
       <c r="BM13" s="9"/>
@@ -2873,16 +3747,16 @@
       <c r="BT13" s="9"/>
       <c r="BU13" s="9"/>
       <c r="BV13" s="9"/>
-      <c r="BW13" s="10"/>
-      <c r="BX13" s="10"/>
-      <c r="BY13" s="10"/>
+      <c r="BW13" s="11"/>
+      <c r="BX13" s="11"/>
+      <c r="BY13" s="11"/>
       <c r="CB13" s="9"/>
       <c r="CC13" s="9"/>
       <c r="CD13" s="9"/>
       <c r="CE13" s="9"/>
       <c r="CG13" s="9"/>
       <c r="CH13" s="9"/>
-      <c r="CI13" s="10"/>
+      <c r="CI13" s="11"/>
       <c r="CJ13" s="9"/>
       <c r="CK13" s="9"/>
       <c r="CL13" s="9"/>
@@ -2909,7 +3783,7 @@
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>70</v>
@@ -2921,36 +3795,79 @@
         <v>15</v>
       </c>
       <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9"/>
-      <c r="AA14" s="9"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="9"/>
-      <c r="AF14" s="9"/>
-      <c r="AG14" s="9"/>
-      <c r="AH14" s="9"/>
-      <c r="AI14" s="9"/>
-      <c r="AK14" s="9"/>
-      <c r="AM14" s="9"/>
-      <c r="AN14" s="9"/>
-      <c r="AO14" s="9"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="P14" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R14" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="T14" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U14" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z14" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA14" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB14" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD14" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE14" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF14" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG14" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH14" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI14" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ14" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK14" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL14" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="AP14" s="9"/>
       <c r="AQ14" s="9"/>
       <c r="AR14" s="9"/>
@@ -2969,8 +3886,8 @@
       <c r="BF14" s="9"/>
       <c r="BG14" s="9"/>
       <c r="BH14" s="9"/>
-      <c r="BI14" s="10"/>
-      <c r="BJ14" s="10"/>
+      <c r="BI14" s="11"/>
+      <c r="BJ14" s="11"/>
       <c r="BK14" s="9"/>
       <c r="BL14" s="9"/>
       <c r="BM14" s="9"/>
@@ -2982,16 +3899,16 @@
       <c r="BT14" s="9"/>
       <c r="BU14" s="9"/>
       <c r="BV14" s="9"/>
-      <c r="BW14" s="10"/>
-      <c r="BX14" s="10"/>
-      <c r="BY14" s="10"/>
+      <c r="BW14" s="11"/>
+      <c r="BX14" s="11"/>
+      <c r="BY14" s="11"/>
       <c r="CB14" s="9"/>
       <c r="CC14" s="9"/>
       <c r="CD14" s="9"/>
       <c r="CE14" s="9"/>
       <c r="CG14" s="9"/>
       <c r="CH14" s="9"/>
-      <c r="CI14" s="10"/>
+      <c r="CI14" s="11"/>
       <c r="CJ14" s="9"/>
       <c r="CK14" s="9"/>
       <c r="CL14" s="9"/>
@@ -3018,7 +3935,7 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>70</v>
@@ -3028,36 +3945,83 @@
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="9"/>
-      <c r="Z15" s="9"/>
-      <c r="AA15" s="9"/>
-      <c r="AB15" s="9"/>
-      <c r="AC15" s="9"/>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="9"/>
-      <c r="AF15" s="9"/>
-      <c r="AG15" s="9"/>
-      <c r="AH15" s="9"/>
-      <c r="AI15" s="9"/>
-      <c r="AK15" s="9"/>
-      <c r="AM15" s="9"/>
-      <c r="AN15" s="9"/>
-      <c r="AO15" s="9"/>
+      <c r="J15" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="L15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="P15" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R15" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="T15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U15" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z15" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA15" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC15" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD15" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE15" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF15" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG15" s="10"/>
+      <c r="AH15" s="10"/>
+      <c r="AI15" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ15" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK15" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL15" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="AP15" s="9"/>
       <c r="AQ15" s="9"/>
       <c r="AR15" s="9"/>
@@ -3076,8 +4040,8 @@
       <c r="BF15" s="9"/>
       <c r="BG15" s="9"/>
       <c r="BH15" s="9"/>
-      <c r="BI15" s="10"/>
-      <c r="BJ15" s="10"/>
+      <c r="BI15" s="11"/>
+      <c r="BJ15" s="11"/>
       <c r="BK15" s="9"/>
       <c r="BL15" s="9"/>
       <c r="BM15" s="9"/>
@@ -3089,16 +4053,16 @@
       <c r="BT15" s="9"/>
       <c r="BU15" s="9"/>
       <c r="BV15" s="9"/>
-      <c r="BW15" s="10"/>
-      <c r="BX15" s="10"/>
-      <c r="BY15" s="10"/>
+      <c r="BW15" s="11"/>
+      <c r="BX15" s="11"/>
+      <c r="BY15" s="11"/>
       <c r="CB15" s="9"/>
       <c r="CC15" s="9"/>
       <c r="CD15" s="9"/>
       <c r="CE15" s="9"/>
       <c r="CG15" s="9"/>
       <c r="CH15" s="9"/>
-      <c r="CI15" s="10"/>
+      <c r="CI15" s="11"/>
       <c r="CJ15" s="9"/>
       <c r="CK15" s="9"/>
       <c r="CL15" s="9"/>
@@ -3126,43 +4090,56 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="G16" s="4" t="n">
         <v>5</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
-      <c r="Z16" s="9"/>
-      <c r="AA16" s="9"/>
-      <c r="AB16" s="9"/>
-      <c r="AC16" s="9"/>
-      <c r="AD16" s="9"/>
-      <c r="AE16" s="9"/>
-      <c r="AF16" s="9"/>
-      <c r="AG16" s="9"/>
-      <c r="AH16" s="9"/>
-      <c r="AI16" s="9"/>
-      <c r="AK16" s="9"/>
-      <c r="AM16" s="9"/>
-      <c r="AN16" s="9"/>
-      <c r="AO16" s="9"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="S16" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="T16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U16" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
+      <c r="AC16" s="10"/>
+      <c r="AD16" s="10"/>
+      <c r="AE16" s="10"/>
+      <c r="AF16" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG16" s="10"/>
+      <c r="AH16" s="10"/>
+      <c r="AI16" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AJ16" s="10"/>
+      <c r="AK16" s="10"/>
+      <c r="AL16" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="AP16" s="9"/>
       <c r="AQ16" s="9"/>
       <c r="AR16" s="9"/>
@@ -3181,8 +4158,8 @@
       <c r="BF16" s="9"/>
       <c r="BG16" s="9"/>
       <c r="BH16" s="9"/>
-      <c r="BI16" s="10"/>
-      <c r="BJ16" s="10"/>
+      <c r="BI16" s="11"/>
+      <c r="BJ16" s="11"/>
       <c r="BK16" s="9"/>
       <c r="BL16" s="9"/>
       <c r="BM16" s="9"/>
@@ -3194,16 +4171,16 @@
       <c r="BT16" s="9"/>
       <c r="BU16" s="9"/>
       <c r="BV16" s="9"/>
-      <c r="BW16" s="10"/>
-      <c r="BX16" s="10"/>
-      <c r="BY16" s="10"/>
+      <c r="BW16" s="11"/>
+      <c r="BX16" s="11"/>
+      <c r="BY16" s="11"/>
       <c r="CB16" s="9"/>
       <c r="CC16" s="9"/>
       <c r="CD16" s="9"/>
       <c r="CE16" s="9"/>
       <c r="CG16" s="9"/>
       <c r="CH16" s="9"/>
-      <c r="CI16" s="10"/>
+      <c r="CI16" s="11"/>
       <c r="CJ16" s="9"/>
       <c r="CK16" s="9"/>
       <c r="CL16" s="9"/>
@@ -3230,7 +4207,7 @@
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>70</v>
@@ -3240,36 +4217,71 @@
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="9"/>
-      <c r="AA17" s="9"/>
-      <c r="AB17" s="9"/>
-      <c r="AC17" s="9"/>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="9"/>
-      <c r="AF17" s="9"/>
-      <c r="AG17" s="9"/>
-      <c r="AH17" s="9"/>
-      <c r="AI17" s="9"/>
-      <c r="AK17" s="9"/>
-      <c r="AM17" s="9"/>
-      <c r="AN17" s="9"/>
-      <c r="AO17" s="9"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="P17" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R17" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="S17" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T17" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="U17" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z17" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA17" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB17" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC17" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD17" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE17" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF17" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AJ17" s="10"/>
+      <c r="AK17" s="10"/>
+      <c r="AL17" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="AP17" s="9"/>
       <c r="AQ17" s="9"/>
       <c r="AR17" s="9"/>
@@ -3288,8 +4300,8 @@
       <c r="BF17" s="9"/>
       <c r="BG17" s="9"/>
       <c r="BH17" s="9"/>
-      <c r="BI17" s="10"/>
-      <c r="BJ17" s="10"/>
+      <c r="BI17" s="11"/>
+      <c r="BJ17" s="11"/>
       <c r="BK17" s="9"/>
       <c r="BL17" s="9"/>
       <c r="BM17" s="9"/>
@@ -3310,7 +4322,7 @@
       <c r="CE17" s="9"/>
       <c r="CG17" s="9"/>
       <c r="CH17" s="9"/>
-      <c r="CI17" s="10"/>
+      <c r="CI17" s="11"/>
       <c r="CJ17" s="9"/>
       <c r="CK17" s="9"/>
       <c r="CL17" s="9"/>
@@ -3337,7 +4349,7 @@
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>70</v>
@@ -3349,36 +4361,87 @@
         <v>20</v>
       </c>
       <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="9"/>
-      <c r="Z18" s="9"/>
-      <c r="AA18" s="9"/>
-      <c r="AB18" s="9"/>
-      <c r="AC18" s="9"/>
-      <c r="AD18" s="9"/>
-      <c r="AE18" s="9"/>
-      <c r="AF18" s="9"/>
-      <c r="AG18" s="9"/>
-      <c r="AH18" s="9"/>
-      <c r="AI18" s="9"/>
-      <c r="AK18" s="9"/>
-      <c r="AM18" s="9"/>
-      <c r="AN18" s="9"/>
-      <c r="AO18" s="9"/>
+      <c r="J18" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L18" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M18" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O18" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R18" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S18" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T18" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="U18" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z18" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA18" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB18" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC18" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD18" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE18" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF18" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH18" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI18" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ18" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK18" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL18" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="AP18" s="9"/>
       <c r="AQ18" s="9"/>
       <c r="AR18" s="9"/>
@@ -3397,8 +4460,8 @@
       <c r="BF18" s="9"/>
       <c r="BG18" s="9"/>
       <c r="BH18" s="9"/>
-      <c r="BI18" s="10"/>
-      <c r="BJ18" s="10"/>
+      <c r="BI18" s="11"/>
+      <c r="BJ18" s="11"/>
       <c r="BK18" s="9"/>
       <c r="BL18" s="9"/>
       <c r="BM18" s="9"/>
@@ -3410,16 +4473,16 @@
       <c r="BT18" s="9"/>
       <c r="BU18" s="9"/>
       <c r="BV18" s="9"/>
-      <c r="BW18" s="10"/>
-      <c r="BX18" s="10"/>
-      <c r="BY18" s="10"/>
+      <c r="BW18" s="11"/>
+      <c r="BX18" s="11"/>
+      <c r="BY18" s="11"/>
       <c r="CB18" s="9"/>
       <c r="CC18" s="9"/>
       <c r="CD18" s="9"/>
       <c r="CE18" s="9"/>
       <c r="CG18" s="9"/>
       <c r="CH18" s="9"/>
-      <c r="CI18" s="10"/>
+      <c r="CI18" s="11"/>
       <c r="CJ18" s="9"/>
       <c r="CK18" s="9"/>
       <c r="CL18" s="9"/>
@@ -3446,7 +4509,7 @@
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>70</v>
@@ -3458,36 +4521,79 @@
         <v>10</v>
       </c>
       <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
-      <c r="AA19" s="9"/>
-      <c r="AB19" s="9"/>
-      <c r="AC19" s="9"/>
-      <c r="AD19" s="9"/>
-      <c r="AE19" s="9"/>
-      <c r="AF19" s="9"/>
-      <c r="AG19" s="9"/>
-      <c r="AH19" s="9"/>
-      <c r="AI19" s="9"/>
-      <c r="AK19" s="9"/>
-      <c r="AM19" s="9"/>
-      <c r="AN19" s="9"/>
-      <c r="AO19" s="9"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O19" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P19" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="R19" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S19" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T19" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="U19" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z19" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB19" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD19" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE19" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF19" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG19" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH19" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI19" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ19" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK19" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL19" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="AP19" s="9"/>
       <c r="AQ19" s="9"/>
       <c r="AR19" s="9"/>
@@ -3506,8 +4612,8 @@
       <c r="BF19" s="9"/>
       <c r="BG19" s="9"/>
       <c r="BH19" s="9"/>
-      <c r="BI19" s="10"/>
-      <c r="BJ19" s="10"/>
+      <c r="BI19" s="11"/>
+      <c r="BJ19" s="11"/>
       <c r="BK19" s="9"/>
       <c r="BL19" s="9"/>
       <c r="BM19" s="9"/>
@@ -3519,16 +4625,16 @@
       <c r="BT19" s="9"/>
       <c r="BU19" s="9"/>
       <c r="BV19" s="9"/>
-      <c r="BW19" s="10"/>
-      <c r="BX19" s="10"/>
-      <c r="BY19" s="10"/>
+      <c r="BW19" s="11"/>
+      <c r="BX19" s="11"/>
+      <c r="BY19" s="11"/>
       <c r="CB19" s="9"/>
       <c r="CC19" s="9"/>
       <c r="CD19" s="9"/>
       <c r="CE19" s="9"/>
       <c r="CG19" s="9"/>
       <c r="CH19" s="9"/>
-      <c r="CI19" s="10"/>
+      <c r="CI19" s="11"/>
       <c r="CJ19" s="9"/>
       <c r="CK19" s="9"/>
       <c r="CL19" s="9"/>
@@ -3555,7 +4661,7 @@
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>70</v>
@@ -3565,36 +4671,67 @@
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="9"/>
-      <c r="AA20" s="9"/>
-      <c r="AB20" s="9"/>
-      <c r="AC20" s="9"/>
-      <c r="AD20" s="9"/>
-      <c r="AE20" s="9"/>
-      <c r="AF20" s="9"/>
-      <c r="AG20" s="9"/>
-      <c r="AH20" s="9"/>
-      <c r="AI20" s="9"/>
-      <c r="AK20" s="9"/>
-      <c r="AM20" s="9"/>
-      <c r="AN20" s="9"/>
-      <c r="AO20" s="9"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S20" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T20" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="U20" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z20" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB20" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD20" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE20" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF20" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG20" s="10"/>
+      <c r="AH20" s="10"/>
+      <c r="AI20" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ20" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK20" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL20" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="AP20" s="9"/>
       <c r="AQ20" s="9"/>
       <c r="AR20" s="9"/>
@@ -3613,8 +4750,8 @@
       <c r="BF20" s="9"/>
       <c r="BG20" s="9"/>
       <c r="BH20" s="9"/>
-      <c r="BI20" s="10"/>
-      <c r="BJ20" s="10"/>
+      <c r="BI20" s="11"/>
+      <c r="BJ20" s="11"/>
       <c r="BK20" s="9"/>
       <c r="BL20" s="9"/>
       <c r="BM20" s="9"/>
@@ -3626,16 +4763,16 @@
       <c r="BT20" s="9"/>
       <c r="BU20" s="9"/>
       <c r="BV20" s="9"/>
-      <c r="BW20" s="10"/>
-      <c r="BX20" s="10"/>
-      <c r="BY20" s="10"/>
+      <c r="BW20" s="11"/>
+      <c r="BX20" s="11"/>
+      <c r="BY20" s="11"/>
       <c r="CB20" s="9"/>
       <c r="CC20" s="9"/>
       <c r="CD20" s="9"/>
       <c r="CE20" s="9"/>
       <c r="CG20" s="9"/>
       <c r="CH20" s="9"/>
-      <c r="CI20" s="10"/>
+      <c r="CI20" s="11"/>
       <c r="CJ20" s="9"/>
       <c r="CK20" s="9"/>
       <c r="CL20" s="9"/>
@@ -3662,7 +4799,7 @@
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>70</v>
@@ -3674,36 +4811,75 @@
         <v>15</v>
       </c>
       <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="9"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="9"/>
-      <c r="AE21" s="9"/>
-      <c r="AF21" s="9"/>
-      <c r="AG21" s="9"/>
-      <c r="AH21" s="9"/>
-      <c r="AI21" s="9"/>
-      <c r="AK21" s="9"/>
-      <c r="AM21" s="9"/>
-      <c r="AN21" s="9"/>
-      <c r="AO21" s="9"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="O21" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="P21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="R21" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="S21" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="T21" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="U21" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z21" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA21" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB21" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC21" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD21" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE21" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF21" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="AG21" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH21" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI21" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AJ21" s="10"/>
+      <c r="AK21" s="10"/>
+      <c r="AL21" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="AP21" s="9"/>
       <c r="AQ21" s="9"/>
       <c r="AR21" s="9"/>
@@ -3722,8 +4898,8 @@
       <c r="BF21" s="9"/>
       <c r="BG21" s="9"/>
       <c r="BH21" s="9"/>
-      <c r="BI21" s="10"/>
-      <c r="BJ21" s="10"/>
+      <c r="BI21" s="11"/>
+      <c r="BJ21" s="11"/>
       <c r="BK21" s="9"/>
       <c r="BL21" s="9"/>
       <c r="BM21" s="9"/>
@@ -3735,16 +4911,16 @@
       <c r="BT21" s="9"/>
       <c r="BU21" s="9"/>
       <c r="BV21" s="9"/>
-      <c r="BW21" s="10"/>
-      <c r="BX21" s="10"/>
-      <c r="BY21" s="10"/>
+      <c r="BW21" s="11"/>
+      <c r="BX21" s="11"/>
+      <c r="BY21" s="11"/>
       <c r="CB21" s="9"/>
       <c r="CC21" s="9"/>
       <c r="CD21" s="9"/>
       <c r="CE21" s="9"/>
       <c r="CG21" s="9"/>
       <c r="CH21" s="9"/>
-      <c r="CI21" s="10"/>
+      <c r="CI21" s="11"/>
       <c r="CJ21" s="9"/>
       <c r="CK21" s="9"/>
       <c r="CL21" s="9"/>
@@ -3771,7 +4947,7 @@
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>70</v>
@@ -3781,36 +4957,67 @@
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="9"/>
-      <c r="Z22" s="9"/>
-      <c r="AA22" s="9"/>
-      <c r="AB22" s="9"/>
-      <c r="AC22" s="9"/>
-      <c r="AD22" s="9"/>
-      <c r="AE22" s="9"/>
-      <c r="AF22" s="9"/>
-      <c r="AG22" s="9"/>
-      <c r="AH22" s="9"/>
-      <c r="AI22" s="9"/>
-      <c r="AK22" s="9"/>
-      <c r="AM22" s="9"/>
-      <c r="AN22" s="9"/>
-      <c r="AO22" s="9"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S22" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="T22" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U22" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z22" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA22" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB22" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC22" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD22" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE22" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF22" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="AG22" s="10"/>
+      <c r="AH22" s="10"/>
+      <c r="AI22" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="AJ22" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK22" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL22" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="AP22" s="9"/>
       <c r="AQ22" s="9"/>
       <c r="AR22" s="9"/>
@@ -3829,8 +5036,8 @@
       <c r="BF22" s="9"/>
       <c r="BG22" s="9"/>
       <c r="BH22" s="9"/>
-      <c r="BI22" s="10"/>
-      <c r="BJ22" s="10"/>
+      <c r="BI22" s="11"/>
+      <c r="BJ22" s="11"/>
       <c r="BK22" s="9"/>
       <c r="BL22" s="9"/>
       <c r="BM22" s="9"/>
@@ -3842,16 +5049,16 @@
       <c r="BT22" s="9"/>
       <c r="BU22" s="9"/>
       <c r="BV22" s="9"/>
-      <c r="BW22" s="10"/>
-      <c r="BX22" s="10"/>
-      <c r="BY22" s="10"/>
+      <c r="BW22" s="11"/>
+      <c r="BX22" s="11"/>
+      <c r="BY22" s="11"/>
       <c r="CB22" s="9"/>
       <c r="CC22" s="9"/>
       <c r="CD22" s="9"/>
       <c r="CE22" s="9"/>
       <c r="CG22" s="9"/>
       <c r="CH22" s="9"/>
-      <c r="CI22" s="10"/>
+      <c r="CI22" s="11"/>
       <c r="CJ22" s="9"/>
       <c r="CK22" s="9"/>
       <c r="CL22" s="9"/>
@@ -3878,46 +5085,77 @@
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="G23" s="4" t="n">
         <v>10</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
-      <c r="Y23" s="9"/>
-      <c r="Z23" s="9"/>
-      <c r="AA23" s="9"/>
-      <c r="AB23" s="9"/>
-      <c r="AC23" s="9"/>
-      <c r="AD23" s="9"/>
-      <c r="AE23" s="9"/>
-      <c r="AF23" s="9"/>
-      <c r="AG23" s="9"/>
-      <c r="AH23" s="9"/>
-      <c r="AI23" s="9"/>
-      <c r="AK23" s="9"/>
-      <c r="AM23" s="9"/>
-      <c r="AN23" s="9"/>
-      <c r="AO23" s="9"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S23" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="T23" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U23" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z23" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA23" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB23" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC23" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD23" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE23" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF23" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG23" s="10"/>
+      <c r="AH23" s="10"/>
+      <c r="AI23" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ23" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK23" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL23" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="AP23" s="9"/>
       <c r="AQ23" s="9"/>
       <c r="AR23" s="9"/>
@@ -3936,8 +5174,8 @@
       <c r="BF23" s="9"/>
       <c r="BG23" s="9"/>
       <c r="BH23" s="9"/>
-      <c r="BI23" s="10"/>
-      <c r="BJ23" s="10"/>
+      <c r="BI23" s="11"/>
+      <c r="BJ23" s="11"/>
       <c r="BK23" s="9"/>
       <c r="BL23" s="9"/>
       <c r="BM23" s="9"/>
@@ -3949,16 +5187,16 @@
       <c r="BT23" s="9"/>
       <c r="BU23" s="9"/>
       <c r="BV23" s="9"/>
-      <c r="BW23" s="10"/>
-      <c r="BX23" s="10"/>
-      <c r="BY23" s="10"/>
+      <c r="BW23" s="11"/>
+      <c r="BX23" s="11"/>
+      <c r="BY23" s="11"/>
       <c r="CB23" s="9"/>
       <c r="CC23" s="9"/>
       <c r="CD23" s="9"/>
       <c r="CE23" s="9"/>
       <c r="CG23" s="9"/>
       <c r="CH23" s="9"/>
-      <c r="CI23" s="10"/>
+      <c r="CI23" s="11"/>
       <c r="CJ23" s="9"/>
       <c r="CK23" s="9"/>
       <c r="CL23" s="9"/>
@@ -3985,7 +5223,7 @@
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>70</v>
@@ -3995,36 +5233,67 @@
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
-      <c r="X24" s="9"/>
-      <c r="Y24" s="9"/>
-      <c r="Z24" s="9"/>
-      <c r="AA24" s="9"/>
-      <c r="AB24" s="9"/>
-      <c r="AC24" s="9"/>
-      <c r="AD24" s="9"/>
-      <c r="AE24" s="9"/>
-      <c r="AF24" s="9"/>
-      <c r="AG24" s="9"/>
-      <c r="AH24" s="9"/>
-      <c r="AI24" s="9"/>
-      <c r="AK24" s="9"/>
-      <c r="AM24" s="9"/>
-      <c r="AN24" s="9"/>
-      <c r="AO24" s="9"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S24" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U24" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z24" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA24" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB24" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC24" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD24" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE24" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF24" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG24" s="10"/>
+      <c r="AH24" s="10"/>
+      <c r="AI24" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ24" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK24" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL24" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="AP24" s="9"/>
       <c r="AQ24" s="9"/>
       <c r="AR24" s="9"/>
@@ -4043,8 +5312,8 @@
       <c r="BF24" s="9"/>
       <c r="BG24" s="9"/>
       <c r="BH24" s="9"/>
-      <c r="BI24" s="10"/>
-      <c r="BJ24" s="10"/>
+      <c r="BI24" s="11"/>
+      <c r="BJ24" s="11"/>
       <c r="BK24" s="9"/>
       <c r="BL24" s="9"/>
       <c r="BM24" s="9"/>
@@ -4056,16 +5325,16 @@
       <c r="BT24" s="9"/>
       <c r="BU24" s="9"/>
       <c r="BV24" s="9"/>
-      <c r="BW24" s="10"/>
-      <c r="BX24" s="10"/>
-      <c r="BY24" s="10"/>
+      <c r="BW24" s="11"/>
+      <c r="BX24" s="11"/>
+      <c r="BY24" s="11"/>
       <c r="CB24" s="9"/>
       <c r="CC24" s="9"/>
       <c r="CD24" s="9"/>
       <c r="CE24" s="9"/>
       <c r="CG24" s="9"/>
       <c r="CH24" s="9"/>
-      <c r="CI24" s="10"/>
+      <c r="CI24" s="11"/>
       <c r="CJ24" s="9"/>
       <c r="CK24" s="9"/>
       <c r="CL24" s="9"/>
@@ -4092,7 +5361,7 @@
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>70</v>
@@ -4104,36 +5373,71 @@
         <v>10</v>
       </c>
       <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
-      <c r="W25" s="9"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="S25" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="T25" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U25" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
       <c r="X25" s="9"/>
-      <c r="Y25" s="9"/>
-      <c r="Z25" s="9"/>
-      <c r="AA25" s="9"/>
-      <c r="AB25" s="9"/>
-      <c r="AC25" s="9"/>
-      <c r="AD25" s="9"/>
-      <c r="AE25" s="9"/>
-      <c r="AF25" s="9"/>
-      <c r="AG25" s="9"/>
-      <c r="AH25" s="9"/>
-      <c r="AI25" s="9"/>
-      <c r="AK25" s="9"/>
-      <c r="AM25" s="9"/>
-      <c r="AN25" s="9"/>
-      <c r="AO25" s="9"/>
+      <c r="Y25" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z25" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA25" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB25" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC25" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD25" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE25" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF25" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG25" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH25" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI25" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ25" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK25" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL25" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="AP25" s="9"/>
       <c r="AQ25" s="9"/>
       <c r="AR25" s="9"/>
@@ -4152,8 +5456,8 @@
       <c r="BF25" s="9"/>
       <c r="BG25" s="9"/>
       <c r="BH25" s="9"/>
-      <c r="BI25" s="10"/>
-      <c r="BJ25" s="10"/>
+      <c r="BI25" s="11"/>
+      <c r="BJ25" s="11"/>
       <c r="BK25" s="9"/>
       <c r="BL25" s="9"/>
       <c r="BM25" s="9"/>
@@ -4165,16 +5469,16 @@
       <c r="BT25" s="9"/>
       <c r="BU25" s="9"/>
       <c r="BV25" s="9"/>
-      <c r="BW25" s="10"/>
-      <c r="BX25" s="10"/>
-      <c r="BY25" s="10"/>
+      <c r="BW25" s="11"/>
+      <c r="BX25" s="11"/>
+      <c r="BY25" s="11"/>
       <c r="CB25" s="9"/>
       <c r="CC25" s="9"/>
       <c r="CD25" s="9"/>
       <c r="CE25" s="9"/>
       <c r="CG25" s="9"/>
       <c r="CH25" s="9"/>
-      <c r="CI25" s="10"/>
+      <c r="CI25" s="11"/>
       <c r="CJ25" s="9"/>
       <c r="CK25" s="9"/>
       <c r="CL25" s="9"/>
@@ -4201,7 +5505,7 @@
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>70</v>
@@ -4214,16 +5518,7 @@
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
       <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
       <c r="U26" s="9"/>
       <c r="V26" s="9"/>
       <c r="W26" s="9"/>
@@ -4238,11 +5533,9 @@
       <c r="AF26" s="9"/>
       <c r="AG26" s="9"/>
       <c r="AH26" s="9"/>
-      <c r="AI26" s="9"/>
+      <c r="AJ26" s="9"/>
       <c r="AK26" s="9"/>
-      <c r="AM26" s="9"/>
-      <c r="AN26" s="9"/>
-      <c r="AO26" s="9"/>
+      <c r="AL26" s="9"/>
       <c r="AP26" s="9"/>
       <c r="AQ26" s="9"/>
       <c r="AR26" s="9"/>
@@ -4261,8 +5554,8 @@
       <c r="BF26" s="9"/>
       <c r="BG26" s="9"/>
       <c r="BH26" s="9"/>
-      <c r="BI26" s="10"/>
-      <c r="BJ26" s="10"/>
+      <c r="BI26" s="11"/>
+      <c r="BJ26" s="11"/>
       <c r="BK26" s="9"/>
       <c r="BL26" s="9"/>
       <c r="BM26" s="9"/>
@@ -4274,16 +5567,16 @@
       <c r="BT26" s="9"/>
       <c r="BU26" s="9"/>
       <c r="BV26" s="9"/>
-      <c r="BW26" s="10"/>
-      <c r="BX26" s="10"/>
-      <c r="BY26" s="10"/>
+      <c r="BW26" s="11"/>
+      <c r="BX26" s="11"/>
+      <c r="BY26" s="11"/>
       <c r="CB26" s="9"/>
       <c r="CC26" s="9"/>
       <c r="CD26" s="9"/>
       <c r="CE26" s="9"/>
       <c r="CG26" s="9"/>
       <c r="CH26" s="9"/>
-      <c r="CI26" s="10"/>
+      <c r="CI26" s="11"/>
       <c r="CJ26" s="9"/>
       <c r="CK26" s="9"/>
       <c r="CL26" s="9"/>
@@ -4310,10 +5603,10 @@
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="G27" s="5" t="n">
         <v>20</v>
@@ -4344,314 +5637,314 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>75</v>
+      <c r="C1" s="12" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>78</v>
+      <c r="A2" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>81</v>
+      <c r="A3" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>78</v>
+      <c r="A4" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>78</v>
+      <c r="A5" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>81</v>
+      <c r="C6" s="14" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>81</v>
+      <c r="A7" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>90</v>
+      <c r="C8" s="14" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>93</v>
+      <c r="A9" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>90</v>
+      <c r="A10" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>81</v>
+      <c r="A11" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>90</v>
+      <c r="A12" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>90</v>
+      <c r="A13" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>93</v>
+      <c r="C14" s="14" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>78</v>
+      <c r="A15" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>81</v>
+      <c r="A16" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>109</v>
+      <c r="A17" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>81</v>
+      <c r="A18" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>81</v>
+      <c r="A19" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>93</v>
+      <c r="C20" s="14" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>81</v>
+      <c r="A21" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>109</v>
+      <c r="A22" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>78</v>
+      <c r="A23" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>90</v>
+      <c r="A24" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>109</v>
+      <c r="A25" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>93</v>
+      <c r="A26" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>81</v>
+      <c r="A27" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>78</v>
+      <c r="A28" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>